<commit_message>
minor changes, test for new ssh key
</commit_message>
<xml_diff>
--- a/lists_for_translator.xlsx
+++ b/lists_for_translator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Me\PycharmProjects\pythonProject_TranslatorMeets Zen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7F2A81-DE6D-4577-9E96-F98CB083C8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0950DAF5-47EB-46B9-B0A3-1CE3B9042570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3384" yWindow="3384" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{A4ABEF32-ABB1-47D8-A5EA-945E0E66EE28}"/>
+    <workbookView xWindow="2268" yWindow="3240" windowWidth="19344" windowHeight="8964" xr2:uid="{A4ABEF32-ABB1-47D8-A5EA-945E0E66EE28}"/>
   </bookViews>
   <sheets>
     <sheet name="управление" sheetId="3" r:id="rId1"/>
@@ -39,18 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
-    <t>идентификаторы</t>
-  </si>
-  <si>
-    <t>перевод</t>
-  </si>
-  <si>
-    <t>полное название элемента</t>
-  </si>
-  <si>
-    <t>тип категории</t>
-  </si>
-  <si>
     <t>факультет</t>
   </si>
   <si>
@@ -183,10 +171,22 @@
     <t>Faculty of Energy and Ecotechnology</t>
   </si>
   <si>
-    <t>актуальность</t>
-  </si>
-  <si>
     <t>нет данных</t>
+  </si>
+  <si>
+    <t>тип категории (name)</t>
+  </si>
+  <si>
+    <t>идентификаторы (id)</t>
+  </si>
+  <si>
+    <t>актуальность (relevance)</t>
+  </si>
+  <si>
+    <t>перевод (items)</t>
+  </si>
+  <si>
+    <t>полное название элемента (keys)</t>
   </si>
 </sst>
 </file>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E246C7-557F-43C9-A2FF-F041F12063BE}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,139 +593,139 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE878CED-5586-44F7-9198-BCEF99FB6A4B}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,128 +753,128 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>